<commit_message>
fixed incosistency of pages
</commit_message>
<xml_diff>
--- a/Test Design Specifications/Search_Nanny_Test_Design_Specification.xlsx
+++ b/Test Design Specifications/Search_Nanny_Test_Design_Specification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Li\Programs\Xampp\htdocs\GrannyNanny\Test Design Specifications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GrannyNanny\Test Design Specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t xml:space="preserve"> Test Design Specification Identifier</t>
   </si>
@@ -197,6 +197,54 @@
   <si>
     <t xml:space="preserve">The UI  follow the same design as all other pages </t>
   </si>
+  <si>
+    <t>No Results found</t>
+  </si>
+  <si>
+    <t>Check if no results found message is displayed with search which doesn’t find anything</t>
+  </si>
+  <si>
+    <t>Search with no filters</t>
+  </si>
+  <si>
+    <t>Check if all results are displayed with empty search</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Няма намерени резултати, моля опитайте отново message appears</t>
+  </si>
+  <si>
+    <t>All the nannies from the DB are displayed as a result</t>
+  </si>
+  <si>
+    <t>Search with non existing and existing criteria</t>
+  </si>
+  <si>
+    <t>Check if something is shown as a result when searching with existing and non existing criteria</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>NR_1</t>
+  </si>
+  <si>
+    <t>SF_1</t>
+  </si>
+  <si>
+    <t>SE_1</t>
+  </si>
+  <si>
+    <t>Search with special symbols</t>
+  </si>
+  <si>
+    <t>SS_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Няма намерени резултати, моля опитайте отново message appears or result containing the searched symbols</t>
+  </si>
+  <si>
+    <t>Try searching with special symbols for example : ". , ' " / ? &lt; &gt; ' } { [ ] ! @ # $ % ^ _ ... "</t>
+  </si>
 </sst>
 </file>
 
@@ -275,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -329,6 +377,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -623,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -660,14 +717,14 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="22" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="20"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -685,10 +742,10 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -749,10 +806,10 @@
       <c r="Y3" s="6"/>
     </row>
     <row r="4" spans="1:25" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
         <v>14</v>
@@ -1237,10 +1294,10 @@
       <c r="Y17" s="6"/>
     </row>
     <row r="18" spans="1:25" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1301,10 +1358,10 @@
       <c r="Y19" s="6"/>
     </row>
     <row r="20" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
-        <v>14</v>
+      <c r="A20" s="22" t="s">
+        <v>59</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1331,12 +1388,18 @@
     </row>
     <row r="21" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1359,11 +1422,10 @@
       <c r="Y21" s="6"/>
     </row>
     <row r="22" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1386,11 +1448,19 @@
       <c r="Y22" s="6"/>
     </row>
     <row r="23" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1412,12 +1482,10 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
     </row>
-    <row r="24" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+    <row r="24" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1440,11 +1508,19 @@
       <c r="Y24" s="6"/>
     </row>
     <row r="25" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1467,7 +1543,9 @@
       <c r="Y25" s="6"/>
     </row>
     <row r="26" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1493,12 +1571,20 @@
       <c r="X26" s="6"/>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+    <row r="27" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>73</v>
+      </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>

</xml_diff>